<commit_message>
Friday Commit 2 SP
</commit_message>
<xml_diff>
--- a/wp5/WP5_Universities Social Private Returns.xlsx
+++ b/wp5/WP5_Universities Social Private Returns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Country\Russia\Data\SEASHELL\SEABYTE\edreru\wp5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FEAFBD-2801-4036-B8AC-D7D3A78FEA5E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB1F866-1435-42AD-87D9-29AC3C257726}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1386,15 +1386,9 @@
     <t>Удмуртский государственный университет</t>
   </si>
   <si>
-    <t>social returns</t>
-  </si>
-  <si>
     <t>private returns</t>
   </si>
   <si>
-    <t>Name of College</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -1417,6 +1411,12 @@
   </si>
   <si>
     <t>LIST OF UNIVERSITIES ARRANGED BY REGION AND INSTITUTION NAME</t>
+  </si>
+  <si>
+    <t>Name of University</t>
+  </si>
+  <si>
+    <t>fiscal returns</t>
   </si>
 </sst>
 </file>
@@ -1543,9 +1543,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A2:J376" totalsRowShown="0" headerRowDxfId="2">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="social returns"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="fiscal returns"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="private returns"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name of College" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name of University" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Region" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total Revenue (in million Rubles)"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Total Paid Fees (in million Rubles)"/>
@@ -1839,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J376"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +1854,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1868,34 +1868,34 @@
     </row>
     <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D2" t="s">
         <v>452</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>